<commit_message>
mod 5 more progs
</commit_message>
<xml_diff>
--- a/webscrapping/Book1.xlsx
+++ b/webscrapping/Book1.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -365,10 +363,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -407,28 +408,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>